<commit_message>
Feature #891 : "Data Log Interface" - Fixed machine finger service form, added servicePort property - Download feature using Batch Process - integrate with third party service(xml parsing)
</commit_message>
<xml_diff>
--- a/inkubator-hrm/src/main/webapp/resources/file_template/finger_swap/finger_swap_captured_upload.xlsx
+++ b/inkubator-hrm/src/main/webapp/resources/file_template/finger_swap/finger_swap_captured_upload.xlsx
@@ -1,8 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15" conformance="strict">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr dateCompatibility="0" filterPrivacy="1" defaultThemeVersion="124226"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
@@ -10,16 +10,11 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="122211"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Nik</t>
   </si>
@@ -27,19 +22,22 @@
     <t>16000079</t>
   </si>
   <si>
+    <t>2015-06-21 17:12:10</t>
+  </si>
+  <si>
+    <t>14000031</t>
+  </si>
+  <si>
+    <t>2015-06-04 08:12:21</t>
+  </si>
+  <si>
     <t>DateTime</t>
-  </si>
-  <si>
-    <t>21-06-2015 17:12:10</t>
-  </si>
-  <si>
-    <t>04-06-2015 08:12:21</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -66,8 +64,8 @@
   </fills>
   <borders count="1">
     <border>
-      <start/>
-      <end/>
+      <left/>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -78,12 +76,10 @@
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -102,7 +98,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://purl.oclc.org/ooxml/drawingml/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -221,22 +217,22 @@
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0%">
-              <a:schemeClr val="phClr">
-                <a:tint val="50%"/>
-                <a:satMod val="300%"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35%">
-              <a:schemeClr val="phClr">
-                <a:tint val="37%"/>
-                <a:satMod val="300%"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100%">
-              <a:schemeClr val="phClr">
-                <a:tint val="15%"/>
-                <a:satMod val="350%"/>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -244,22 +240,22 @@
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0%">
-              <a:schemeClr val="phClr">
-                <a:shade val="51%"/>
-                <a:satMod val="130%"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80%">
-              <a:schemeClr val="phClr">
-                <a:shade val="93%"/>
-                <a:satMod val="130%"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100%">
-              <a:schemeClr val="phClr">
-                <a:shade val="94%"/>
-                <a:satMod val="135%"/>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
@@ -270,8 +266,8 @@
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
-              <a:shade val="95%"/>
-              <a:satMod val="105%"/>
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
             </a:schemeClr>
           </a:solidFill>
           <a:prstDash val="solid"/>
@@ -294,7 +290,7 @@
           <a:effectLst>
             <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38%"/>
+                <a:alpha val="38000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -303,7 +299,7 @@
           <a:effectLst>
             <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="35%"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -312,7 +308,7 @@
           <a:effectLst>
             <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="35%"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -335,47 +331,47 @@
         </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0%">
-              <a:schemeClr val="phClr">
-                <a:tint val="40%"/>
-                <a:satMod val="350%"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40%">
-              <a:schemeClr val="phClr">
-                <a:tint val="45%"/>
-                <a:shade val="99%"/>
-                <a:satMod val="350%"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100%">
-              <a:schemeClr val="phClr">
-                <a:shade val="20%"/>
-                <a:satMod val="255%"/>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50%" t="-80%" r="50%" b="180%"/>
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
-            <a:gs pos="0%">
-              <a:schemeClr val="phClr">
-                <a:tint val="80%"/>
-                <a:satMod val="300%"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100%">
-              <a:schemeClr val="phClr">
-                <a:shade val="30%"/>
-                <a:satMod val="200%"/>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50%" t="50%" r="50%" b="50%"/>
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -387,17 +383,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="16" style="3" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -405,20 +401,20 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="4">
-        <v>14000014</v>
+      <c r="A3" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>4</v>

</xml_diff>